<commit_message>
Dialog now working with SMS + email + meetings
</commit_message>
<xml_diff>
--- a/nlc/ipa-web-nlc_training.xlsx
+++ b/nlc/ipa-web-nlc_training.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curated" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Saved" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">original!$A$1:$E$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">original!$A$1:$E$116</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="230">
   <si>
     <t>Input</t>
   </si>
@@ -684,13 +684,43 @@
   </si>
   <si>
     <t>Call schedule</t>
+  </si>
+  <si>
+    <t>send text message</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <t>send text message to *</t>
+  </si>
+  <si>
+    <t>send sms</t>
+  </si>
+  <si>
+    <t>send sms to *</t>
+  </si>
+  <si>
+    <t>send a message to *</t>
+  </si>
+  <si>
+    <t>send an sms to *</t>
+  </si>
+  <si>
+    <t>send a text message to *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text a message to </t>
+  </si>
+  <si>
+    <t>text a message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -714,6 +744,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -732,7 +767,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -848,11 +883,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -910,6 +966,16 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -967,6 +1033,16 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1296,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B159"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2010,107 +2086,107 @@
     <row r="71" spans="1:2">
       <c r="A71" t="str">
         <f>original!A72</f>
-        <v>2+2</v>
+        <v>send text message</v>
       </c>
       <c r="B71" t="str">
         <f>original!B72</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="str">
         <f>original!A73</f>
-        <v>5*5/12</v>
+        <v>send text message to *</v>
       </c>
       <c r="B72" t="str">
         <f>original!B73</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="str">
         <f>original!A74</f>
-        <v>122*254/5</v>
+        <v>send sms</v>
       </c>
       <c r="B73" t="str">
         <f>original!B74</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="str">
         <f>original!A75</f>
-        <v>66/34</v>
+        <v>send sms to *</v>
       </c>
       <c r="B74" t="str">
         <f>original!B75</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="str">
         <f>original!A76</f>
-        <v>2-5*5</v>
+        <v>send a message to *</v>
       </c>
       <c r="B75" t="str">
         <f>original!B76</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="str">
         <f>original!A77</f>
-        <v>(2*5)*5-(9/8)</v>
+        <v>send an sms to *</v>
       </c>
       <c r="B76" t="str">
         <f>original!B77</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="str">
         <f>original!A78</f>
-        <v>123*984/2</v>
+        <v>send a text message to *</v>
       </c>
       <c r="B77" t="str">
         <f>original!B78</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="str">
         <f>original!A79</f>
-        <v>(234-567)/453</v>
+        <v>send text message</v>
       </c>
       <c r="B78" t="str">
         <f>original!B79</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="str">
         <f>original!A80</f>
-        <v>255*255</v>
+        <v xml:space="preserve">text a message to </v>
       </c>
       <c r="B79" t="str">
         <f>original!B80</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="str">
         <f>original!A81</f>
-        <v>122*122</v>
+        <v>text a message</v>
       </c>
       <c r="B80" t="str">
         <f>original!B81</f>
-        <v>respond-calculation-numeric</v>
+        <v>action-sms-create</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="str">
         <f>original!A82</f>
-        <v>8^2</v>
+        <v>2+2</v>
       </c>
       <c r="B81" t="str">
         <f>original!B82</f>
@@ -2120,7 +2196,7 @@
     <row r="82" spans="1:2">
       <c r="A82" t="str">
         <f>original!A83</f>
-        <v>12^100</v>
+        <v>5*5/12</v>
       </c>
       <c r="B82" t="str">
         <f>original!B83</f>
@@ -2130,7 +2206,7 @@
     <row r="83" spans="1:2">
       <c r="A83" t="str">
         <f>original!A84</f>
-        <v>12*12</v>
+        <v>122*254/5</v>
       </c>
       <c r="B83" t="str">
         <f>original!B84</f>
@@ -2140,7 +2216,7 @@
     <row r="84" spans="1:2">
       <c r="A84" t="str">
         <f>original!A85</f>
-        <v>133*133</v>
+        <v>66/34</v>
       </c>
       <c r="B84" t="str">
         <f>original!B85</f>
@@ -2150,7 +2226,7 @@
     <row r="85" spans="1:2">
       <c r="A85" t="str">
         <f>original!A86</f>
-        <v>2^8</v>
+        <v>2-5*5</v>
       </c>
       <c r="B85" t="str">
         <f>original!B86</f>
@@ -2160,107 +2236,107 @@
     <row r="86" spans="1:2">
       <c r="A86" t="str">
         <f>original!A87</f>
-        <v>5 feet to inches</v>
+        <v>(2*5)*5-(9/8)</v>
       </c>
       <c r="B86" t="str">
         <f>original!B87</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="str">
         <f>original!A88</f>
-        <v>5 inches to feet</v>
+        <v>123*984/2</v>
       </c>
       <c r="B87" t="str">
         <f>original!B88</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="str">
         <f>original!A89</f>
-        <v>10 quarts to gallons</v>
+        <v>(234-567)/453</v>
       </c>
       <c r="B88" t="str">
         <f>original!B89</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="str">
         <f>original!A90</f>
-        <v>5 hours to days</v>
+        <v>255*255</v>
       </c>
       <c r="B89" t="str">
         <f>original!B90</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="str">
         <f>original!A91</f>
-        <v>10 mins to seconds</v>
+        <v>122*122</v>
       </c>
       <c r="B90" t="str">
         <f>original!B91</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="str">
         <f>original!A92</f>
-        <v>10 seconds to mins</v>
+        <v>8^2</v>
       </c>
       <c r="B91" t="str">
         <f>original!B92</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="str">
         <f>original!A93</f>
-        <v>5 meters to miles</v>
+        <v>12^100</v>
       </c>
       <c r="B92" t="str">
         <f>original!B93</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="str">
         <f>original!A94</f>
-        <v>500 miles to kilometers</v>
+        <v>12*12</v>
       </c>
       <c r="B93" t="str">
         <f>original!B94</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="str">
         <f>original!A95</f>
-        <v>5000 feet to miles</v>
+        <v>133*133</v>
       </c>
       <c r="B94" t="str">
         <f>original!B95</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="str">
         <f>original!A96</f>
-        <v>1 mile to kilometers</v>
+        <v>2^8</v>
       </c>
       <c r="B95" t="str">
         <f>original!B96</f>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="str">
         <f>original!A97</f>
-        <v>10 kilometers to miles</v>
+        <v>5 feet to inches</v>
       </c>
       <c r="B96" t="str">
         <f>original!B97</f>
@@ -2270,7 +2346,7 @@
     <row r="97" spans="1:2">
       <c r="A97" t="str">
         <f>original!A98</f>
-        <v>10 kgs to pounds</v>
+        <v>5 inches to feet</v>
       </c>
       <c r="B97" t="str">
         <f>original!B98</f>
@@ -2280,7 +2356,7 @@
     <row r="98" spans="1:2">
       <c r="A98" t="str">
         <f>original!A99</f>
-        <v>10 grams to ounces</v>
+        <v>10 quarts to gallons</v>
       </c>
       <c r="B98" t="str">
         <f>original!B99</f>
@@ -2290,7 +2366,7 @@
     <row r="99" spans="1:2">
       <c r="A99" t="str">
         <f>original!A100</f>
-        <v>20 ounces to pounds</v>
+        <v>5 hours to days</v>
       </c>
       <c r="B99" t="str">
         <f>original!B100</f>
@@ -2300,7 +2376,7 @@
     <row r="100" spans="1:2">
       <c r="A100" t="str">
         <f>original!A101</f>
-        <v>20 pounts to grams</v>
+        <v>10 mins to seconds</v>
       </c>
       <c r="B100" t="str">
         <f>original!B101</f>
@@ -2310,7 +2386,7 @@
     <row r="101" spans="1:2">
       <c r="A101" t="str">
         <f>original!A102</f>
-        <v>1 oz to grams</v>
+        <v>10 seconds to mins</v>
       </c>
       <c r="B101" t="str">
         <f>original!B102</f>
@@ -2320,197 +2396,197 @@
     <row r="102" spans="1:2">
       <c r="A102" t="str">
         <f>original!A103</f>
-        <v>Do you know a good joke?</v>
+        <v>5 meters to miles</v>
       </c>
       <c r="B102" t="str">
         <f>original!B103</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="str">
         <f>original!A104</f>
-        <v>Tell me a funny joke</v>
+        <v>500 miles to kilometers</v>
       </c>
       <c r="B103" t="str">
         <f>original!B104</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="str">
         <f>original!A105</f>
-        <v>Tell me a joke</v>
+        <v>5000 feet to miles</v>
       </c>
       <c r="B104" t="str">
         <f>original!B105</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="str">
         <f>original!A106</f>
-        <v>Tell me a story</v>
+        <v>1 mile to kilometers</v>
       </c>
       <c r="B105" t="str">
         <f>original!B106</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="str">
         <f>original!A107</f>
-        <v>Tell me something funny?</v>
+        <v>10 kilometers to miles</v>
       </c>
       <c r="B106" t="str">
         <f>original!B107</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="str">
         <f>original!A108</f>
-        <v>Make me laugh</v>
+        <v>10 kgs to pounds</v>
       </c>
       <c r="B107" t="str">
         <f>original!B108</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="str">
         <f>original!A109</f>
-        <v>Make a joke</v>
+        <v>10 grams to ounces</v>
       </c>
       <c r="B108" t="str">
         <f>original!B109</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="str">
         <f>original!A110</f>
-        <v>Know any good jokes</v>
+        <v>20 ounces to pounds</v>
       </c>
       <c r="B109" t="str">
         <f>original!B110</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="str">
         <f>original!A111</f>
-        <v>Tell me another joke</v>
+        <v>20 pounts to grams</v>
       </c>
       <c r="B110" t="str">
         <f>original!B111</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="str">
         <f>original!A112</f>
-        <v>1 plus 1</v>
+        <v>1 oz to grams</v>
       </c>
       <c r="B111" t="str">
         <f>original!B112</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-calculation-conversion</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="str">
         <f>original!A113</f>
-        <v>1+1</v>
+        <v>Do you know a good joke?</v>
       </c>
       <c r="B112" t="str">
         <f>original!B113</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="str">
         <f>original!A114</f>
-        <v>1+1=?</v>
+        <v>Tell me a funny joke</v>
       </c>
       <c r="B113" t="str">
         <f>original!B114</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="str">
         <f>original!A115</f>
-        <v>10 plus 10</v>
+        <v>Tell me a joke</v>
       </c>
       <c r="B114" t="str">
         <f>original!B115</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="str">
         <f>original!A116</f>
-        <v>10 + 10 =</v>
+        <v>Tell me a story</v>
       </c>
       <c r="B115" t="str">
         <f>original!B116</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="str">
         <f>original!A117</f>
-        <v>10+10=?</v>
+        <v>Tell me something funny?</v>
       </c>
       <c r="B116" t="str">
         <f>original!B117</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="str">
         <f>original!A118</f>
-        <v>100 minus 10</v>
+        <v>Make me laugh</v>
       </c>
       <c r="B117" t="str">
         <f>original!B118</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="str">
         <f>original!A119</f>
-        <v>5 plus five</v>
+        <v>Make a joke</v>
       </c>
       <c r="B118" t="str">
         <f>original!B119</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="str">
         <f>original!A120</f>
-        <v>a million plus a billion?</v>
+        <v>Know any good jokes</v>
       </c>
       <c r="B119" t="str">
         <f>original!B120</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="str">
         <f>original!A121</f>
-        <v>infinity</v>
+        <v>Tell me another joke</v>
       </c>
       <c r="B120" t="str">
         <f>original!B121</f>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="str">
         <f>original!A122</f>
-        <v>infinity / infinity</v>
+        <v>1 plus 1</v>
       </c>
       <c r="B121" t="str">
         <f>original!B122</f>
@@ -2520,7 +2596,7 @@
     <row r="122" spans="1:2">
       <c r="A122" t="str">
         <f>original!A123</f>
-        <v>infinity divided by zero</v>
+        <v>1+1</v>
       </c>
       <c r="B122" t="str">
         <f>original!B123</f>
@@ -2530,7 +2606,7 @@
     <row r="123" spans="1:2">
       <c r="A123" t="str">
         <f>original!A124</f>
-        <v>infinity/infinity</v>
+        <v>1+1=?</v>
       </c>
       <c r="B123" t="str">
         <f>original!B124</f>
@@ -2540,7 +2616,7 @@
     <row r="124" spans="1:2">
       <c r="A124" t="str">
         <f>original!A125</f>
-        <v>What is * divided by zero?</v>
+        <v>10 plus 10</v>
       </c>
       <c r="B124" t="str">
         <f>original!B125</f>
@@ -2550,7 +2626,7 @@
     <row r="125" spans="1:2">
       <c r="A125" t="str">
         <f>original!A126</f>
-        <v>What is 1/0?</v>
+        <v>10 + 10 =</v>
       </c>
       <c r="B125" t="str">
         <f>original!B126</f>
@@ -2560,7 +2636,7 @@
     <row r="126" spans="1:2">
       <c r="A126" t="str">
         <f>original!A127</f>
-        <v>What is 1+1?</v>
+        <v>10+10=?</v>
       </c>
       <c r="B126" t="str">
         <f>original!B127</f>
@@ -2570,7 +2646,7 @@
     <row r="127" spans="1:2">
       <c r="A127" t="str">
         <f>original!A128</f>
-        <v>What is 2+2</v>
+        <v>100 minus 10</v>
       </c>
       <c r="B127" t="str">
         <f>original!B128</f>
@@ -2580,7 +2656,7 @@
     <row r="128" spans="1:2">
       <c r="A128" t="str">
         <f>original!A129</f>
-        <v>what is nine plus fourteen?</v>
+        <v>5 plus five</v>
       </c>
       <c r="B128" t="str">
         <f>original!B129</f>
@@ -2590,310 +2666,410 @@
     <row r="129" spans="1:2">
       <c r="A129" t="str">
         <f>original!A130</f>
-        <v>'agk4'3k'p0f23k</v>
+        <v>a million plus a billion?</v>
       </c>
       <c r="B129" t="str">
         <f>original!B130</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="str">
         <f>original!A131</f>
-        <v>@#$@%#fwweWf wef W#Rjlwf34;</v>
+        <v>infinity</v>
       </c>
       <c r="B130" t="str">
         <f>original!B131</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="str">
         <f>original!A132</f>
-        <v>292-494f4</v>
+        <v>infinity / infinity</v>
       </c>
       <c r="B131" t="str">
         <f>original!B132</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="str">
         <f>original!A133</f>
-        <v>ajfskdw49urwe0w3ufiwel</v>
+        <v>infinity divided by zero</v>
       </c>
       <c r="B132" t="str">
         <f>original!B133</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="str">
         <f>original!A134</f>
-        <v>asd f efwefjkw jkl</v>
+        <v>infinity/infinity</v>
       </c>
       <c r="B133" t="str">
         <f>original!B134</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="str">
         <f>original!A135</f>
-        <v>aslkdjal</v>
+        <v>What is * divided by zero?</v>
       </c>
       <c r="B134" t="str">
         <f>original!B135</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="str">
         <f>original!A136</f>
-        <v>jklfadsk23450923u u9q3uf203 9u</v>
+        <v>What is 1/0?</v>
       </c>
       <c r="B135" t="str">
         <f>original!B136</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="str">
         <f>original!A137</f>
-        <v>sadjka; jakls;djfakls; dfjasd ;flk</v>
+        <v>What is 1+1?</v>
       </c>
       <c r="B136" t="str">
         <f>original!B137</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="str">
         <f>original!A138</f>
-        <v>blah blah blah</v>
+        <v>What is 2+2</v>
       </c>
       <c r="B137" t="str">
         <f>original!B138</f>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="str">
         <f>original!A139</f>
-        <v>Is god real?</v>
+        <v>what is nine plus fourteen?</v>
       </c>
       <c r="B138" t="str">
         <f>original!B139</f>
-        <v>respond-off-topic-philosophy</v>
+        <v>respond-off-topic-math</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="str">
         <f>original!A140</f>
-        <v>What is the meaning of life?</v>
+        <v>'agk4'3k'p0f23k</v>
       </c>
       <c r="B139" t="str">
         <f>original!B140</f>
-        <v>respond-off-topic-philosophy</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="str">
         <f>original!A141</f>
-        <v>why do we die?</v>
+        <v>@#$@%#fwweWf wef W#Rjlwf34;</v>
       </c>
       <c r="B140" t="str">
         <f>original!B141</f>
-        <v>respond-off-topic-philosophy</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="str">
         <f>original!A142</f>
-        <v>why do we live?</v>
+        <v>292-494f4</v>
       </c>
       <c r="B141" t="str">
         <f>original!B142</f>
-        <v>respond-off-topic-philosophy</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="str">
         <f>original!A143</f>
-        <v>what is * in light years?</v>
+        <v>ajfskdw49urwe0w3ufiwel</v>
       </c>
       <c r="B142" t="str">
         <f>original!B143</f>
-        <v>respond-off-topic-science</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="str">
         <f>original!A144</f>
-        <v>I'm tired</v>
+        <v>asd f efwefjkw jkl</v>
       </c>
       <c r="B143" t="str">
         <f>original!B144</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="str">
         <f>original!A145</f>
-        <v>I'm drunk</v>
+        <v>aslkdjal</v>
       </c>
       <c r="B144" t="str">
         <f>original!B145</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="str">
         <f>original!A146</f>
-        <v>I'm naked</v>
+        <v>jklfadsk23450923u u9q3uf203 9u</v>
       </c>
       <c r="B145" t="str">
         <f>original!B146</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="str">
         <f>original!A147</f>
-        <v>Talk dirty to me</v>
+        <v>sadjka; jakls;djfakls; dfjasd ;flk</v>
       </c>
       <c r="B146" t="str">
         <f>original!B147</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="str">
         <f>original!A148</f>
-        <v>I love you</v>
+        <v>blah blah blah</v>
       </c>
       <c r="B147" t="str">
         <f>original!B148</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="str">
         <f>original!A149</f>
-        <v>Ask me a question</v>
+        <v>Is god real?</v>
       </c>
       <c r="B148" t="str">
         <f>original!B149</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-philosophy</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="str">
         <f>original!A150</f>
-        <v>i had a terrible day!</v>
+        <v>What is the meaning of life?</v>
       </c>
       <c r="B149" t="str">
         <f>original!B150</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-philosophy</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="str">
         <f>original!A151</f>
-        <v>I'm sad</v>
+        <v>why do we die?</v>
       </c>
       <c r="B150" t="str">
         <f>original!B151</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-philosophy</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="str">
         <f>original!A152</f>
-        <v>my computer broke!</v>
+        <v>why do we live?</v>
       </c>
       <c r="B151" t="str">
         <f>original!B152</f>
-        <v>respond-off-topic-user-focus</v>
+        <v>respond-off-topic-philosophy</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="str">
         <f>original!A153</f>
-        <v>Do you have eyes?</v>
+        <v>what is * in light years?</v>
       </c>
       <c r="B152" t="str">
         <f>original!B153</f>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-science</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="str">
         <f>original!A154</f>
-        <v>where is your hardware?</v>
+        <v>I'm tired</v>
       </c>
       <c r="B153" t="str">
         <f>original!B154</f>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-user-focus</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="str">
         <f>original!A155</f>
-        <v>are you happy?</v>
+        <v>I'm drunk</v>
       </c>
       <c r="B154" t="str">
         <f>original!B155</f>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-user-focus</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="str">
         <f>original!A156</f>
-        <v>Do you follow the three laws of robotics?</v>
+        <v>I'm naked</v>
       </c>
       <c r="B155" t="str">
         <f>original!B156</f>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-user-focus</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="str">
         <f>original!A157</f>
-        <v>Do you have feelings?</v>
+        <v>Talk dirty to me</v>
       </c>
       <c r="B156" t="str">
         <f>original!B157</f>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-user-focus</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="str">
         <f>original!A158</f>
-        <v>How old are you</v>
+        <v>I love you</v>
       </c>
       <c r="B157" t="str">
         <f>original!B158</f>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-user-focus</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="str">
         <f>original!A159</f>
-        <v>What is your favorite color?</v>
+        <v>Ask me a question</v>
       </c>
       <c r="B158" t="str">
         <f>original!B159</f>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-user-focus</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="str">
         <f>original!A160</f>
-        <v>What's your favourite animal?</v>
+        <v>i had a terrible day!</v>
       </c>
       <c r="B159" t="str">
         <f>original!B160</f>
+        <v>respond-off-topic-user-focus</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="str">
+        <f>original!A161</f>
+        <v>I'm sad</v>
+      </c>
+      <c r="B160" t="str">
+        <f>original!B161</f>
+        <v>respond-off-topic-user-focus</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="str">
+        <f>original!A162</f>
+        <v>my computer broke!</v>
+      </c>
+      <c r="B161" t="str">
+        <f>original!B162</f>
+        <v>respond-off-topic-user-focus</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="str">
+        <f>original!A163</f>
+        <v>Do you have eyes?</v>
+      </c>
+      <c r="B162" t="str">
+        <f>original!B163</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="str">
+        <f>original!A164</f>
+        <v>where is your hardware?</v>
+      </c>
+      <c r="B163" t="str">
+        <f>original!B164</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="str">
+        <f>original!A165</f>
+        <v>are you happy?</v>
+      </c>
+      <c r="B164" t="str">
+        <f>original!B165</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="str">
+        <f>original!A166</f>
+        <v>Do you follow the three laws of robotics?</v>
+      </c>
+      <c r="B165" t="str">
+        <f>original!B166</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="str">
+        <f>original!A167</f>
+        <v>Do you have feelings?</v>
+      </c>
+      <c r="B166" t="str">
+        <f>original!B167</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="str">
+        <f>original!A168</f>
+        <v>How old are you</v>
+      </c>
+      <c r="B167" t="str">
+        <f>original!B168</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="str">
+        <f>original!A169</f>
+        <v>What is your favorite color?</v>
+      </c>
+      <c r="B168" t="str">
+        <f>original!B169</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="str">
+        <f>original!A170</f>
+        <v>What's your favourite animal?</v>
+      </c>
+      <c r="B169" t="str">
+        <f>original!B170</f>
         <v>respond-off-topic-watson-focus</v>
       </c>
     </row>
@@ -2910,10 +3086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A170" sqref="A170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4095,7 +4271,7 @@
         <v>136</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B72" si="2">CONCATENATE(C66,"-",D66,"-",E66)</f>
+        <f t="shared" ref="B66:B82" si="2">CONCATENATE(C66,"-",D66,"-",E66)</f>
         <v>action-meeting-create</v>
       </c>
       <c r="C66" t="s">
@@ -4185,7 +4361,7 @@
         <v>141</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE(C71,"-",D71,"-",E71)</f>
         <v>action-meeting-create</v>
       </c>
       <c r="C71" t="s">
@@ -4198,194 +4374,194 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
-      <c r="A72" t="s">
+    <row r="72" spans="1:5" ht="17">
+      <c r="A72" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" ref="B72:B81" si="3">CONCATENATE(C72,"-",D72,"-",E72)</f>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="17">
+      <c r="A73" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>221</v>
+      </c>
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>223</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>224</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>221</v>
+      </c>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>221</v>
+      </c>
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>226</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>221</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>227</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>221</v>
+      </c>
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>220</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>221</v>
+      </c>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>228</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>221</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>229</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="3"/>
+        <v>action-sms-create</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>221</v>
+      </c>
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
         <v>186</v>
       </c>
-      <c r="B72" t="str">
+      <c r="B82" t="str">
         <f t="shared" si="2"/>
         <v>respond-calculation-numeric</v>
       </c>
-      <c r="C72" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" t="s">
-        <v>184</v>
-      </c>
-      <c r="E72" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" t="s">
-        <v>187</v>
-      </c>
-      <c r="B73" t="str">
-        <f t="shared" ref="B73:B86" si="3">CONCATENATE(C73,"-",D73,"-",E73)</f>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C73" t="s">
-        <v>92</v>
-      </c>
-      <c r="D73" t="s">
-        <v>184</v>
-      </c>
-      <c r="E73" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" t="s">
-        <v>188</v>
-      </c>
-      <c r="B74" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C74" t="s">
-        <v>92</v>
-      </c>
-      <c r="D74" t="s">
-        <v>184</v>
-      </c>
-      <c r="E74" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" t="s">
-        <v>189</v>
-      </c>
-      <c r="B75" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C75" t="s">
-        <v>92</v>
-      </c>
-      <c r="D75" t="s">
-        <v>184</v>
-      </c>
-      <c r="E75" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" t="s">
-        <v>190</v>
-      </c>
-      <c r="B76" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C76" t="s">
-        <v>92</v>
-      </c>
-      <c r="D76" t="s">
-        <v>184</v>
-      </c>
-      <c r="E76" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" t="s">
-        <v>191</v>
-      </c>
-      <c r="B77" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C77" t="s">
-        <v>92</v>
-      </c>
-      <c r="D77" t="s">
-        <v>184</v>
-      </c>
-      <c r="E77" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" t="s">
-        <v>192</v>
-      </c>
-      <c r="B78" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C78" t="s">
-        <v>92</v>
-      </c>
-      <c r="D78" t="s">
-        <v>184</v>
-      </c>
-      <c r="E78" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" t="s">
-        <v>193</v>
-      </c>
-      <c r="B79" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C79" t="s">
-        <v>92</v>
-      </c>
-      <c r="D79" t="s">
-        <v>184</v>
-      </c>
-      <c r="E79" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" t="s">
-        <v>194</v>
-      </c>
-      <c r="B80" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C80" t="s">
-        <v>92</v>
-      </c>
-      <c r="D80" t="s">
-        <v>184</v>
-      </c>
-      <c r="E80" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" t="s">
-        <v>195</v>
-      </c>
-      <c r="B81" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
-      <c r="C81" t="s">
-        <v>92</v>
-      </c>
-      <c r="D81" t="s">
-        <v>184</v>
-      </c>
-      <c r="E81" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" t="s">
-        <v>196</v>
-      </c>
-      <c r="B82" t="str">
-        <f t="shared" si="3"/>
-        <v>respond-calculation-numeric</v>
-      </c>
       <c r="C82" t="s">
         <v>92</v>
       </c>
@@ -4398,10 +4574,10 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B83:B96" si="4">CONCATENATE(C83,"-",D83,"-",E83)</f>
         <v>respond-calculation-numeric</v>
       </c>
       <c r="C83" t="s">
@@ -4416,10 +4592,10 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>respond-calculation-numeric</v>
       </c>
       <c r="C84" t="s">
@@ -4434,10 +4610,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>respond-calculation-numeric</v>
       </c>
       <c r="C85" t="s">
@@ -4452,10 +4628,10 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>respond-calculation-numeric</v>
       </c>
       <c r="C86" t="s">
@@ -4470,11 +4646,11 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" ref="B87:B103" si="4">CONCATENATE(C87,"-",D87,"-",E87)</f>
-        <v>respond-calculation-conversion</v>
+        <f t="shared" si="4"/>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C87" t="s">
         <v>92</v>
@@ -4483,16 +4659,16 @@
         <v>184</v>
       </c>
       <c r="E87" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B88" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C88" t="s">
         <v>92</v>
@@ -4501,16 +4677,16 @@
         <v>184</v>
       </c>
       <c r="E88" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C89" t="s">
         <v>92</v>
@@ -4519,16 +4695,16 @@
         <v>184</v>
       </c>
       <c r="E89" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B90" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C90" t="s">
         <v>92</v>
@@ -4537,16 +4713,16 @@
         <v>184</v>
       </c>
       <c r="E90" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B91" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C91" t="s">
         <v>92</v>
@@ -4555,16 +4731,16 @@
         <v>184</v>
       </c>
       <c r="E91" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B92" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C92" t="s">
         <v>92</v>
@@ -4573,16 +4749,16 @@
         <v>184</v>
       </c>
       <c r="E92" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C93" t="s">
         <v>92</v>
@@ -4591,16 +4767,16 @@
         <v>184</v>
       </c>
       <c r="E93" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C94" t="s">
         <v>92</v>
@@ -4609,16 +4785,16 @@
         <v>184</v>
       </c>
       <c r="E94" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C95" t="s">
         <v>92</v>
@@ -4627,16 +4803,16 @@
         <v>184</v>
       </c>
       <c r="E95" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="4"/>
-        <v>respond-calculation-conversion</v>
+        <v>respond-calculation-numeric</v>
       </c>
       <c r="C96" t="s">
         <v>92</v>
@@ -4645,15 +4821,15 @@
         <v>184</v>
       </c>
       <c r="E96" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B97:B113" si="5">CONCATENATE(C97,"-",D97,"-",E97)</f>
         <v>respond-calculation-conversion</v>
       </c>
       <c r="C97" t="s">
@@ -4668,10 +4844,10 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>respond-calculation-conversion</v>
       </c>
       <c r="C98" t="s">
@@ -4686,10 +4862,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>respond-calculation-conversion</v>
       </c>
       <c r="C99" t="s">
@@ -4704,10 +4880,10 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>respond-calculation-conversion</v>
       </c>
       <c r="C100" t="s">
@@ -4722,10 +4898,10 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>respond-calculation-conversion</v>
       </c>
       <c r="C101" t="s">
@@ -4740,10 +4916,10 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>respond-calculation-conversion</v>
       </c>
       <c r="C102" t="s">
@@ -4758,191 +4934,191 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" si="4"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <f t="shared" si="5"/>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C103" t="s">
         <v>92</v>
       </c>
       <c r="D103" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E103" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" ref="B104:B126" si="5">CONCATENATE(C104,"-",D104,"-",E104)</f>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <f t="shared" si="5"/>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C104" t="s">
         <v>92</v>
       </c>
       <c r="D104" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E104" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>53</v>
+        <v>210</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C105" t="s">
         <v>92</v>
       </c>
       <c r="D105" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E105" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>83</v>
+        <v>211</v>
       </c>
       <c r="B106" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C106" t="s">
         <v>92</v>
       </c>
       <c r="D106" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E106" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C107" t="s">
         <v>92</v>
       </c>
       <c r="D107" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E107" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C108" t="s">
         <v>92</v>
       </c>
       <c r="D108" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E108" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C109" t="s">
         <v>92</v>
       </c>
       <c r="D109" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E109" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="B110" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C110" t="s">
         <v>92</v>
       </c>
       <c r="D110" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E110" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="B111" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-joke-or-riddle</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C111" t="s">
         <v>92</v>
       </c>
       <c r="D111" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E111" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>54</v>
+        <v>217</v>
       </c>
       <c r="B112" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <v>respond-calculation-conversion</v>
       </c>
       <c r="C112" t="s">
         <v>92</v>
       </c>
       <c r="D112" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="E112" t="s">
-        <v>98</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>55</v>
+        <v>177</v>
       </c>
       <c r="B113" t="str">
         <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C113" t="s">
         <v>92</v>
@@ -4951,16 +5127,16 @@
         <v>93</v>
       </c>
       <c r="E113" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>56</v>
+        <v>179</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" ref="B114:B136" si="6">CONCATENATE(C114,"-",D114,"-",E114)</f>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C114" t="s">
         <v>92</v>
@@ -4969,16 +5145,16 @@
         <v>93</v>
       </c>
       <c r="E114" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" si="6"/>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C115" t="s">
         <v>92</v>
@@ -4987,16 +5163,16 @@
         <v>93</v>
       </c>
       <c r="E115" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" si="6"/>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C116" t="s">
         <v>92</v>
@@ -5005,16 +5181,16 @@
         <v>93</v>
       </c>
       <c r="E116" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>58</v>
+        <v>180</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" si="6"/>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C117" t="s">
         <v>92</v>
@@ -5023,16 +5199,16 @@
         <v>93</v>
       </c>
       <c r="E117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>59</v>
+        <v>178</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" si="6"/>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C118" t="s">
         <v>92</v>
@@ -5041,16 +5217,16 @@
         <v>93</v>
       </c>
       <c r="E118" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" si="6"/>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C119" t="s">
         <v>92</v>
@@ -5059,16 +5235,16 @@
         <v>93</v>
       </c>
       <c r="E119" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" si="6"/>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C120" t="s">
         <v>92</v>
@@ -5077,16 +5253,16 @@
         <v>93</v>
       </c>
       <c r="E120" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>62</v>
+        <v>183</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="5"/>
-        <v>respond-off-topic-math</v>
+        <f t="shared" si="6"/>
+        <v>respond-off-topic-joke-or-riddle</v>
       </c>
       <c r="C121" t="s">
         <v>92</v>
@@ -5095,15 +5271,15 @@
         <v>93</v>
       </c>
       <c r="E121" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>respond-off-topic-math</v>
       </c>
       <c r="C122" t="s">
@@ -5118,10 +5294,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>respond-off-topic-math</v>
       </c>
       <c r="C123" t="s">
@@ -5136,10 +5312,10 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>respond-off-topic-math</v>
       </c>
       <c r="C124" t="s">
@@ -5154,10 +5330,10 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B125" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>respond-off-topic-math</v>
       </c>
       <c r="C125" t="s">
@@ -5172,10 +5348,10 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>respond-off-topic-math</v>
       </c>
       <c r="C126" t="s">
@@ -5190,10 +5366,10 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" ref="B127:B158" si="6">CONCATENATE(C127,"-",D127,"-",E127)</f>
+        <f t="shared" si="6"/>
         <v>respond-off-topic-math</v>
       </c>
       <c r="C127" t="s">
@@ -5208,7 +5384,7 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B128" t="str">
         <f t="shared" si="6"/>
@@ -5226,7 +5402,7 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B129" t="str">
         <f t="shared" si="6"/>
@@ -5244,11 +5420,11 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B130" t="str">
         <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C130" t="s">
         <v>92</v>
@@ -5257,16 +5433,16 @@
         <v>93</v>
       </c>
       <c r="E130" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B131" t="str">
         <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C131" t="s">
         <v>92</v>
@@ -5275,16 +5451,16 @@
         <v>93</v>
       </c>
       <c r="E131" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B132" t="str">
         <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C132" t="s">
         <v>92</v>
@@ -5293,16 +5469,16 @@
         <v>93</v>
       </c>
       <c r="E132" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B133" t="str">
         <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C133" t="s">
         <v>92</v>
@@ -5311,16 +5487,16 @@
         <v>93</v>
       </c>
       <c r="E133" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B134" t="str">
         <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C134" t="s">
         <v>92</v>
@@ -5329,16 +5505,16 @@
         <v>93</v>
       </c>
       <c r="E134" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B135" t="str">
         <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C135" t="s">
         <v>92</v>
@@ -5347,16 +5523,16 @@
         <v>93</v>
       </c>
       <c r="E135" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B136" t="str">
         <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C136" t="s">
         <v>92</v>
@@ -5365,16 +5541,16 @@
         <v>93</v>
       </c>
       <c r="E136" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B137" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <f t="shared" ref="B137:B168" si="7">CONCATENATE(C137,"-",D137,"-",E137)</f>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C137" t="s">
         <v>92</v>
@@ -5383,16 +5559,16 @@
         <v>93</v>
       </c>
       <c r="E137" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B138" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-nonsense-input</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C138" t="s">
         <v>92</v>
@@ -5401,16 +5577,16 @@
         <v>93</v>
       </c>
       <c r="E138" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B139" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-philosophy</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-math</v>
       </c>
       <c r="C139" t="s">
         <v>92</v>
@@ -5419,16 +5595,16 @@
         <v>93</v>
       </c>
       <c r="E139" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B140" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-philosophy</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C140" t="s">
         <v>92</v>
@@ -5437,16 +5613,16 @@
         <v>93</v>
       </c>
       <c r="E140" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B141" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-philosophy</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C141" t="s">
         <v>92</v>
@@ -5455,16 +5631,16 @@
         <v>93</v>
       </c>
       <c r="E141" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B142" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-philosophy</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C142" t="s">
         <v>92</v>
@@ -5473,16 +5649,16 @@
         <v>93</v>
       </c>
       <c r="E142" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B143" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-science</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C143" t="s">
         <v>92</v>
@@ -5491,16 +5667,16 @@
         <v>93</v>
       </c>
       <c r="E143" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B144" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C144" t="s">
         <v>92</v>
@@ -5509,16 +5685,16 @@
         <v>93</v>
       </c>
       <c r="E144" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B145" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C145" t="s">
         <v>92</v>
@@ -5527,16 +5703,16 @@
         <v>93</v>
       </c>
       <c r="E145" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B146" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C146" t="s">
         <v>92</v>
@@ -5545,16 +5721,16 @@
         <v>93</v>
       </c>
       <c r="E146" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B147" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C147" t="s">
         <v>92</v>
@@ -5563,16 +5739,16 @@
         <v>93</v>
       </c>
       <c r="E147" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B148" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-nonsense-input</v>
       </c>
       <c r="C148" t="s">
         <v>92</v>
@@ -5581,16 +5757,16 @@
         <v>93</v>
       </c>
       <c r="E148" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B149" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-philosophy</v>
       </c>
       <c r="C149" t="s">
         <v>92</v>
@@ -5599,16 +5775,16 @@
         <v>93</v>
       </c>
       <c r="E149" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B150" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-philosophy</v>
       </c>
       <c r="C150" t="s">
         <v>92</v>
@@ -5617,16 +5793,16 @@
         <v>93</v>
       </c>
       <c r="E150" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B151" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-philosophy</v>
       </c>
       <c r="C151" t="s">
         <v>92</v>
@@ -5635,16 +5811,16 @@
         <v>93</v>
       </c>
       <c r="E151" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B152" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-user-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-philosophy</v>
       </c>
       <c r="C152" t="s">
         <v>92</v>
@@ -5653,16 +5829,16 @@
         <v>93</v>
       </c>
       <c r="E152" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="B153" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-watson-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-science</v>
       </c>
       <c r="C153" t="s">
         <v>92</v>
@@ -5671,16 +5847,16 @@
         <v>93</v>
       </c>
       <c r="E153" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B154" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-watson-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
       </c>
       <c r="C154" t="s">
         <v>92</v>
@@ -5689,16 +5865,16 @@
         <v>93</v>
       </c>
       <c r="E154" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B155" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-watson-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
       </c>
       <c r="C155" t="s">
         <v>92</v>
@@ -5707,16 +5883,16 @@
         <v>93</v>
       </c>
       <c r="E155" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B156" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-watson-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
       </c>
       <c r="C156" t="s">
         <v>92</v>
@@ -5725,16 +5901,16 @@
         <v>93</v>
       </c>
       <c r="E156" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B157" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-watson-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
       </c>
       <c r="C157" t="s">
         <v>92</v>
@@ -5743,16 +5919,16 @@
         <v>93</v>
       </c>
       <c r="E157" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B158" t="str">
-        <f t="shared" si="6"/>
-        <v>respond-off-topic-watson-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
       </c>
       <c r="C158" t="s">
         <v>92</v>
@@ -5761,16 +5937,16 @@
         <v>93</v>
       </c>
       <c r="E158" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B159" t="str">
-        <f t="shared" ref="B159:B160" si="7">CONCATENATE(C159,"-",D159,"-",E159)</f>
-        <v>respond-off-topic-watson-focus</v>
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
       </c>
       <c r="C159" t="s">
         <v>92</v>
@@ -5779,16 +5955,16 @@
         <v>93</v>
       </c>
       <c r="E159" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B160" t="str">
         <f t="shared" si="7"/>
-        <v>respond-off-topic-watson-focus</v>
+        <v>respond-off-topic-user-focus</v>
       </c>
       <c r="C160" t="s">
         <v>92</v>
@@ -5797,11 +5973,191 @@
         <v>93</v>
       </c>
       <c r="E160" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>81</v>
+      </c>
+      <c r="B161" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
+      </c>
+      <c r="C161" t="s">
+        <v>92</v>
+      </c>
+      <c r="D161" t="s">
+        <v>93</v>
+      </c>
+      <c r="E161" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>82</v>
+      </c>
+      <c r="B162" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-user-focus</v>
+      </c>
+      <c r="C162" t="s">
+        <v>92</v>
+      </c>
+      <c r="D162" t="s">
+        <v>93</v>
+      </c>
+      <c r="E162" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>84</v>
+      </c>
+      <c r="B163" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C163" t="s">
+        <v>92</v>
+      </c>
+      <c r="D163" t="s">
+        <v>93</v>
+      </c>
+      <c r="E163" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>85</v>
+      </c>
+      <c r="B164" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C164" t="s">
+        <v>92</v>
+      </c>
+      <c r="D164" t="s">
+        <v>93</v>
+      </c>
+      <c r="E164" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>86</v>
+      </c>
+      <c r="B165" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C165" t="s">
+        <v>92</v>
+      </c>
+      <c r="D165" t="s">
+        <v>93</v>
+      </c>
+      <c r="E165" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>87</v>
+      </c>
+      <c r="B166" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C166" t="s">
+        <v>92</v>
+      </c>
+      <c r="D166" t="s">
+        <v>93</v>
+      </c>
+      <c r="E166" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>88</v>
+      </c>
+      <c r="B167" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C167" t="s">
+        <v>92</v>
+      </c>
+      <c r="D167" t="s">
+        <v>93</v>
+      </c>
+      <c r="E167" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>89</v>
+      </c>
+      <c r="B168" t="str">
+        <f t="shared" si="7"/>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C168" t="s">
+        <v>92</v>
+      </c>
+      <c r="D168" t="s">
+        <v>93</v>
+      </c>
+      <c r="E168" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>90</v>
+      </c>
+      <c r="B169" t="str">
+        <f t="shared" ref="B169:B170" si="8">CONCATENATE(C169,"-",D169,"-",E169)</f>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C169" t="s">
+        <v>92</v>
+      </c>
+      <c r="D169" t="s">
+        <v>93</v>
+      </c>
+      <c r="E169" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>91</v>
+      </c>
+      <c r="B170" t="str">
+        <f t="shared" si="8"/>
+        <v>respond-off-topic-watson-focus</v>
+      </c>
+      <c r="C170" t="s">
+        <v>92</v>
+      </c>
+      <c r="D170" t="s">
+        <v>93</v>
+      </c>
+      <c r="E170" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E106">
+  <autoFilter ref="A1:E116">
     <sortState ref="A2:E163">
       <sortCondition ref="B1:B163"/>
     </sortState>

</xml_diff>